<commit_message>
Update for first draft of showing visualization
</commit_message>
<xml_diff>
--- a/doc/messagesDefinition.xlsx
+++ b/doc/messagesDefinition.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\builds\dds-launchpad-iiot-poc-psg-pub\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7F3FA34-D95A-4A09-8F03-E17FDBD2BED9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21315" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="messageSchema" sheetId="1" r:id="rId1"/>
     <sheet name="sample01" sheetId="2" r:id="rId2"/>
+    <sheet name="sample02" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
   <si>
     <t>timestamp</t>
   </si>
@@ -147,9 +149,6 @@
     <t>[302,142,102,302,303,304,305,306,307,308]</t>
   </si>
   <si>
-    <t>[303,132,106,347,236,237,238,2239,240,241]</t>
-  </si>
-  <si>
     <t>[111,241,206,207,208,209,210,211,212,213]</t>
   </si>
   <si>
@@ -166,12 +165,15 @@
   </si>
   <si>
     <t>[112,205,230,217,202,203,204,205,206,207]</t>
+  </si>
+  <si>
+    <t>[303,132,106,347,236,237,238,223,240,241]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,27 +525,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.3046875" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" customWidth="1"/>
+    <col min="9" max="9" width="26.84375" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -575,7 +577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -607,7 +609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -621,7 +623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -641,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -661,7 +663,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -678,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -695,31 +697,31 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I16" s="1"/>
     </row>
   </sheetData>
@@ -728,27 +730,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.3046875" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="45.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="63.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" customWidth="1"/>
+    <col min="9" max="9" width="45.53515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="63.15234375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -780,7 +782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -812,7 +814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -826,7 +828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -846,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -866,7 +868,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -883,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -900,7 +902,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -929,7 +931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>10000</v>
       </c>
@@ -958,7 +960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>20000</v>
       </c>
@@ -987,7 +989,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>5000</v>
       </c>
@@ -1013,10 +1015,10 @@
         <v>35</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10000</v>
       </c>
@@ -1042,10 +1044,10 @@
         <v>36</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>20000</v>
       </c>
@@ -1071,10 +1073,10 @@
         <v>37</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>15000</v>
       </c>
@@ -1100,10 +1102,10 @@
         <v>38</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>10000</v>
       </c>
@@ -1129,10 +1131,10 @@
         <v>39</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>20000</v>
       </c>
@@ -1155,13 +1157,13 @@
         <v>10</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1170,4 +1172,299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8977B2-AAE5-4B3C-96B4-E86BDEB69204}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.61328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="36.69140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>4096</v>
+      </c>
+      <c r="G5">
+        <v>4096</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J5" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>233</v>
+      </c>
+      <c r="G6">
+        <v>2700</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>358</v>
+      </c>
+      <c r="G7">
+        <v>3600</v>
+      </c>
+      <c r="I7" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J7" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>250</v>
+      </c>
+      <c r="G8">
+        <v>3000</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>10000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>2500</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>10000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>180</v>
+      </c>
+      <c r="G10">
+        <v>3500</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I14" s="3"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I15" s="3"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I16" s="3"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed first round of visualization for PSG Vibration Project
</commit_message>
<xml_diff>
--- a/doc/messagesDefinition.xlsx
+++ b/doc/messagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\builds\dds-launchpad-iiot-poc-psg-pub\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7F3FA34-D95A-4A09-8F03-E17FDBD2BED9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{317CBE65-0D82-45B6-9F7F-121C3D461FA8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
   <si>
     <t>timestamp</t>
   </si>
@@ -89,9 +89,6 @@
     <t>auto</t>
   </si>
   <si>
-    <t>client01</t>
-  </si>
-  <si>
     <t>emu18</t>
   </si>
   <si>
@@ -134,40 +131,61 @@
     <t>[110,203,228,215,200,201,202,203,204,205]</t>
   </si>
   <si>
-    <t>[201,131,111,112,113,114,115,116,117,118]</t>
-  </si>
-  <si>
-    <t>[301,141,101,301,302,303,304,305,306,307]</t>
-  </si>
-  <si>
-    <t>[302,131,105,346,235,236,237,238,239,240]</t>
-  </si>
-  <si>
-    <t>[202,132,111,112,113,114,115,116,117,118]</t>
-  </si>
-  <si>
-    <t>[302,142,102,302,303,304,305,306,307,308]</t>
-  </si>
-  <si>
-    <t>[111,241,206,207,208,209,210,211,212,213]</t>
-  </si>
-  <si>
-    <t>[101,201,221,226,227,228,229,230,231,232]</t>
-  </si>
-  <si>
-    <t>[111,204,229,216,201,202,203,204,205,206]</t>
-  </si>
-  <si>
-    <t>[112,242,207,208,209,210,211,212,213,214]</t>
-  </si>
-  <si>
-    <t>[102,202,222,227,228,229,230,231,232,233]</t>
-  </si>
-  <si>
-    <t>[112,205,230,217,202,203,204,205,206,207]</t>
-  </si>
-  <si>
-    <t>[303,132,106,347,236,237,238,223,240,241]</t>
+    <t>[110,240,205,206,207,208,209,210,211,212,110,240,205,206,217,208,219,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,111,194,132,222,223,216,211,212,110,241,115,226,227,208,209,210,211,212,110,240,205,126,207,201,109,210,211,112,113,241,105,206,107,201,219,122,211,112]</t>
+  </si>
+  <si>
+    <t>[100,200,220,225,226,227,228,229,230,231,110,240,205,156,117,128,229,210,212,212,131,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,222,285,232,113,134,225,135,162,221,241,225,116,237,108,209,210,211,212,110,240,205,226,217,202,229,210,221,213,245,242,125,206,107,228,109,123,111,112]</t>
+  </si>
+  <si>
+    <t>[111,241,206,207,208,209,210,211,212,213,110,240,205,236,237,148,249,210,214,212,118,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,244,161,144,185,131,225,157,282,123,242,245,126,157,108,209,210,211,212,110,240,205,216,106,204,109,210,241,215,114,244,145,206,107,305,201,126,131,205]</t>
+  </si>
+  <si>
+    <t>[101,201,221,226,227,228,229,230,231,232,110,240,205,126,147,158,159,210,215,212,118,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,255,252,255,176,124,134,148,192,234,243,135,216,167,108,209,210,211,212,110,240,205,107,117,126,203,210,251,116,162,245,155,206,107,127,204,127,151,120]</t>
+  </si>
+  <si>
+    <t>[111,204,229,216,201,202,203,204,205,207,110,240,205,126,247,158,249,210,113,212,148,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,166,114,156,167,135,243,239,172,225,243,245,116,177,208,209,210,211,212,110,240,205,243,135,125,119,210,261,117,234,246,165,206,107,238,178,128,141,117]</t>
+  </si>
+  <si>
+    <t>[112,242,207,208,209,210,211,212,213,214,110,240,205,216,137,158,139,210,212,212,158,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,177,253,267,158,236,132,121,162,116,244,135,226,157,108,209,210,211,212,110,240,205,217,231,128,156,210,271,218,229,247,175,206,107,216,212,129,161,200]</t>
+  </si>
+  <si>
+    <t>[102,202,222,227,228,229,230,231,232,233,110,240,205,106,227,228,229,210,111,212,168,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,188,145,166,249,127,141,130,152,125,244,225,106,167,108,209,210,211,212,110,240,205,109,247,228,157,210,281,119,112,248,185,206,107,128,231,113,171,201]</t>
+  </si>
+  <si>
+    <t>[112,205,230,217,202,203,204,205,206,207,110,240,205,106,217,218,119,210,210,212,179,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,295,236,275,238,219,250,241,222,236,243,215,216,157,208,209,210,211,212,110,240,205,236,137,208,158,210,291,210,103,249,195,206,107,236,203,210,181,232]</t>
+  </si>
+  <si>
+    <t>psgpoc</t>
+  </si>
+  <si>
+    <t>[110,203,228,215,200,201,202,203,204,205,110,240,205,146,127,238,139,210,113,212,120,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,210,211,212,110,240,205,206,207,208,209,110,211,212,110,240,133,176,243,214,223,136,246,172,232,242,135,106,147,208,209,210,211,212,110,240,205,125,205,203,219,210,231,114,253,243,135,206,107,108,218,124,121,207,200]</t>
+  </si>
+  <si>
+    <t>[110,111,112,113,114,115,116,117,190,191,192,193,194,195,196,197,210,211,212,213,214,215,216,217,310,311,312,313,314,315,316,317,410,411,412,413,414,415,416,417,610,611,612,613,614,615,616,617,610,611,612,613,614,615,616,617,810,811,812,813,814,815,816,817,910,911,912,913,914,915,916,917,1110,1111,1112,1113,1114,1115,1116,1117,1210,1211,1212,1213,1214,1215,1216,1217,1310,1311,1312,1313,1314,1315,1316,1317]</t>
+  </si>
+  <si>
+    <t>[100,300,301,302,303,304,305,306,499,500,501,502,503,504,505,506,699,700,701,702,703,704,705,706,899,900,901,902,903,904,905,906,1100,1300,1301,1302,1303,1304,1305,1306,2100,2300,2301,2302,2303,2304,2305,2306,3100,3300,3301,3302,3303,3304,3305,3306,3100,4300,4301,4302,4303,4304,4305,4306,5100,5300,5301,5302,5303,5304,5305,5306,6100,6300,6301,6302,6303,6304,6305,6306,6400,6410,6401,6402,6403,6404,6405,6406,6500,6510,6501,6502,6503,6504,6505,6506]</t>
+  </si>
+  <si>
+    <t>[104,345,234,235,236,237,238,239,1104,1345,1234,1235,1236,1237,1238,1239,2104,2345,2234,2235,2236,2237,2238,2239,3104,3345,3234,3235,3236,3237,3238,3239,4104,4345,4234,4235,4236,4237,4238,4239,5104,5345,5234,5235,5236,5237,5238,5239,6104,6345,6234,6235,6236,6237,6238,6239,7104,7345,7234,7235,7236,7237,7238,7239,8104,8345,8234,8235,8236,8237,8238,8239,9104,9345,9234,9235,9236,9237,9238,9239,9404,9445,9434,9435,9436,9437,9438,9439,9504,9545,9534,9535,9536,9537,9538,9539]</t>
+  </si>
+  <si>
+    <t>[111,112,113,114,115,116,117,118,119,120,121,122,123,124,125,126,127,128,129,130,131,116,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146,147,148,140,150,151,152,153,154,155,156,157,158,159,160,161,162,163,164,165,166,167,168,169,170,171,172,173,174,175,176,177,178,179,180,181,182,183,184,185,186,187,188,189,190,191,192,193,194,195,196,197,198,199,200,201,202,203,204,205,206,207,208,209]</t>
+  </si>
+  <si>
+    <t>[101,301,302,303,304,305,306,307,300,301,302,303,304,305,306,307,310,311,312,313,314,315,316,317,320,321,321,322,323,324,325,326,130,331,332,333,334,335,336,337,340,341,342,343,344,345,346,347,350,351,352,353,354,355,356,357,360,361,362,363,364,365,366,367,370,371,372,373,374,375,376,377,380,381,382,383,384,385,386,387,376,377,380,381,382,383,384,385,386,387,396,397,398,399,400,403,404,405,406,407]</t>
+  </si>
+  <si>
+    <t>[1105,1346,1235,1236,1237,1238,1239,1240,2105,2346,2235,2236,2237,2238,2239,2240,3105,3346,3235,3236,3237,3238,3239,3240,4105,4346,4235,4236,4237,4238,4239,4240,5105,5346,5235,5236,5237,5238,5239,5240,6105,6346,6235,6236,6237,6238,6239,6240,7105,7346,7235,7236,7237,7238,7239,7240,8105,8346,8235,8236,8237,8238,8239,8240,9105,9346,9235,9236,9237,9238,9239,9240,9805,9846,9835,9836,9837,9838,9839,9840,9939,9940,9905,9946,9935,9936,9937,9938,9939,9941,9239,9942,9985,9986,9998,9998,9999,9991,9902,9903]</t>
+  </si>
+  <si>
+    <t>[2111,2112,2113,2114,2115,2116,2117,2118,3111,3112,3113,3114,3115,3116,3117,3118,4111,4112,4113,4114,4115,4116,4117,4118,5111,5112,5113,5114,5115,5116,5117,5118,6111,6112,6113,6114,6115,6116,6117,6118,7111,7112,7113,7114,7115,7116,7117,7118,8111,8112,8113,8114,8115,8116,8117,8118,9111,9112,9113,9114,9115,9116,9117,9118,9211,9212,9213,9214,9215,9216,9217,9218,9311,9312,9313,9314,9315,9316,9317,9318,9417,9418,9411,9412,9413,9414,9415,9416,9417,9418,9517,9518,9511,9512,9513,9514,9515,9516,9517,9518]</t>
+  </si>
+  <si>
+    <t>[3102,3302,3303,3304,3305,3306,3307,3308,4102,4302,4303,4304,4305,4306,4307,4308,5102,5302,5303,5304,5305,5306,5307,5308,6102,6302,6303,6304,6305,6306,6307,6308,7102,7302,7303,7304,7305,7306,7307,7308,8102,8302,8303,8304,8305,8306,8307,8308,9102,9302,9303,9304,9305,9306,9307,9308,9402,9412,9403,9404,9405,9406,9407,9408,9501,9502,9503,9504,9505,9506,9507,9508,9601,9602,9603,9604,9605,9606,9607,9608,9667,9668,9661,9662,9663,9664,9665,9666,9667,9668,9707,9708,9701,9702,9703,9704,9705,9706,9707,9788]</t>
+  </si>
+  <si>
+    <t>[106,107,108,109,110,111,112,113,114,115,116,117,118,119,120,121,122,123,124,125,126,127,128,129,130,131,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146,147,148,149,150,151,152,153,154,155,156,157,158,159,160,161,162,163,164,165,166,167,168,169,170,171,172,173,174,175,176,177,178,179,180,181,182,183,184,185,186,187,188,189,190,191,192,193,194,195,196,197,198,199,200,201,202,203,204,205]</t>
   </si>
 </sst>
 </file>
@@ -529,7 +547,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -541,8 +559,8 @@
     <col min="6" max="6" width="12.53515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="16.53515625" customWidth="1"/>
-    <col min="9" max="9" width="26.84375" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="26.84375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -553,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -571,10 +589,10 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -603,10 +621,10 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -657,10 +675,10 @@
         <v>1000</v>
       </c>
       <c r="I5">
+        <v>255</v>
+      </c>
+      <c r="J5">
         <v>10000</v>
-      </c>
-      <c r="J5">
-        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -691,38 +709,38 @@
         <v>3600</v>
       </c>
       <c r="I7">
+        <v>255</v>
+      </c>
+      <c r="J7">
         <v>10000</v>
       </c>
-      <c r="J7">
-        <v>255</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -733,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -746,8 +764,8 @@
     <col min="6" max="6" width="12.53515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="16.53515625" customWidth="1"/>
-    <col min="9" max="9" width="45.53515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="63.15234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="255.69140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="182.53515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -758,13 +776,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -776,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -808,10 +826,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -862,10 +880,10 @@
         <v>1000</v>
       </c>
       <c r="I5" s="2">
+        <v>255</v>
+      </c>
+      <c r="J5" s="2">
         <v>10000</v>
-      </c>
-      <c r="J5" s="2">
-        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -896,10 +914,10 @@
         <v>3600</v>
       </c>
       <c r="I7" s="2">
+        <v>255</v>
+      </c>
+      <c r="J7" s="2">
         <v>10000</v>
-      </c>
-      <c r="J7" s="2">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
@@ -907,13 +925,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <v>250</v>
@@ -922,13 +940,13 @@
         <v>3000</v>
       </c>
       <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
@@ -936,13 +954,13 @@
         <v>10000</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>200</v>
@@ -951,13 +969,13 @@
         <v>2500</v>
       </c>
       <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>32</v>
+        <v>100</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
@@ -965,13 +983,13 @@
         <v>20000</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>180</v>
@@ -980,13 +998,13 @@
         <v>3500</v>
       </c>
       <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
@@ -994,13 +1012,13 @@
         <v>5000</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>200</v>
@@ -1009,13 +1027,13 @@
         <v>3001</v>
       </c>
       <c r="H11">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
@@ -1023,13 +1041,13 @@
         <v>10000</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12">
         <v>176</v>
@@ -1038,13 +1056,13 @@
         <v>2501</v>
       </c>
       <c r="H12">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>41</v>
+        <v>100</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -1052,13 +1070,13 @@
         <v>20000</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13">
         <v>201</v>
@@ -1067,13 +1085,13 @@
         <v>3501</v>
       </c>
       <c r="H13">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>42</v>
+        <v>100</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -1081,13 +1099,13 @@
         <v>15000</v>
       </c>
       <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14">
         <v>235</v>
@@ -1096,13 +1114,13 @@
         <v>3002</v>
       </c>
       <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>43</v>
+        <v>100</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -1110,13 +1128,13 @@
         <v>10000</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <v>202</v>
@@ -1125,13 +1143,13 @@
         <v>2502</v>
       </c>
       <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
@@ -1139,13 +1157,13 @@
         <v>20000</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>165</v>
@@ -1154,13 +1172,13 @@
         <v>3503</v>
       </c>
       <c r="H16">
-        <v>10</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>45</v>
+        <v>100</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
@@ -1179,7 +1197,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1203,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1221,10 +1239,10 @@
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -1253,10 +1271,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -1309,10 +1327,10 @@
         <v>1000</v>
       </c>
       <c r="I5" s="2">
+        <v>255</v>
+      </c>
+      <c r="J5" s="2">
         <v>10000</v>
-      </c>
-      <c r="J5" s="2">
-        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -1343,10 +1361,10 @@
         <v>3600</v>
       </c>
       <c r="I7" s="2">
+        <v>255</v>
+      </c>
+      <c r="J7" s="2">
         <v>10000</v>
-      </c>
-      <c r="J7" s="2">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
@@ -1354,13 +1372,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <v>250</v>
@@ -1371,11 +1389,11 @@
       <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
+      <c r="J8" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
@@ -1383,13 +1401,13 @@
         <v>10000</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>200</v>
@@ -1400,11 +1418,11 @@
       <c r="H9">
         <v>10</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>32</v>
+      <c r="J9" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
@@ -1412,13 +1430,13 @@
         <v>10000</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>180</v>
@@ -1429,36 +1447,36 @@
       <c r="H10">
         <v>10</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>34</v>
+      <c r="J10" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I11" s="3"/>
-      <c r="J11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I14" s="3"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I15" s="3"/>
-      <c r="J15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I16" s="3"/>
-      <c r="J16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.4">
       <c r="I17" s="2"/>

</xml_diff>

<commit_message>
Latest set of changes for PSG poc and platform (user login and user registration)
</commit_message>
<xml_diff>
--- a/doc/messagesDefinition.xlsx
+++ b/doc/messagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\builds\dds-launchpad-iiot-poc-psg-pub\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{317CBE65-0D82-45B6-9F7F-121C3D461FA8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE28A7AF-EBD5-4B93-BEEE-772AB856036E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
   <si>
     <t>timestamp</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>[106,107,108,109,110,111,112,113,114,115,116,117,118,119,120,121,122,123,124,125,126,127,128,129,130,131,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146,147,148,149,150,151,152,153,154,155,156,157,158,159,160,161,162,163,164,165,166,167,168,169,170,171,172,173,174,175,176,177,178,179,180,181,182,183,184,185,186,187,188,189,190,191,192,193,194,195,196,197,198,199,200,201,202,203,204,205]</t>
+  </si>
+  <si>
+    <t>sensorIndex</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -556,14 +559,15 @@
     <col min="2" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="14.3046875" customWidth="1"/>
     <col min="5" max="5" width="20.15234375" customWidth="1"/>
-    <col min="6" max="6" width="12.53515625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.53515625" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="26.84375" customWidth="1"/>
+    <col min="6" max="6" width="13.53515625" customWidth="1"/>
+    <col min="7" max="7" width="12.53515625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="16.53515625" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
+    <col min="11" max="11" width="26.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -580,22 +584,25 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -621,13 +628,16 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -641,7 +651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -660,87 +670,93 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="F5">
-        <v>4096</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>4096</v>
       </c>
       <c r="H5">
+        <v>4096</v>
+      </c>
+      <c r="I5">
         <v>1000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>255</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>233</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2700</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>358</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3600</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>255</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J16" s="1"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -749,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -761,14 +777,15 @@
     <col min="2" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="14.3046875" customWidth="1"/>
     <col min="5" max="5" width="20.15234375" customWidth="1"/>
-    <col min="6" max="6" width="12.53515625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.53515625" customWidth="1"/>
-    <col min="9" max="9" width="255.69140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="182.53515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.53515625" customWidth="1"/>
+    <col min="7" max="7" width="12.53515625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="16.53515625" customWidth="1"/>
+    <col min="10" max="10" width="255.69140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="182.53515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -785,22 +802,25 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -825,14 +845,17 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
+      <c r="I2" t="s">
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -846,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -859,68 +882,74 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="F5">
-        <v>4096</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>4096</v>
       </c>
       <c r="H5">
+        <v>4096</v>
+      </c>
+      <c r="I5">
         <v>1000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>255</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>233</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2700</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
       <c r="J6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>358</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3600</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>255</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -934,22 +963,25 @@
         <v>26</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>250</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>3000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>100</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>10000</v>
       </c>
@@ -963,22 +995,25 @@
         <v>27</v>
       </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>200</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2500</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>100</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>20000</v>
       </c>
@@ -992,22 +1027,25 @@
         <v>26</v>
       </c>
       <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
         <v>180</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3500</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>100</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>5000</v>
       </c>
@@ -1021,22 +1059,25 @@
         <v>27</v>
       </c>
       <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
         <v>200</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>3001</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>100</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10000</v>
       </c>
@@ -1050,22 +1091,25 @@
         <v>27</v>
       </c>
       <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
         <v>176</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2501</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>100</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>20000</v>
       </c>
@@ -1079,22 +1123,25 @@
         <v>26</v>
       </c>
       <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
         <v>201</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>3501</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>100</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>15000</v>
       </c>
@@ -1108,22 +1155,25 @@
         <v>27</v>
       </c>
       <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
         <v>235</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>3002</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>100</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>10000</v>
       </c>
@@ -1137,22 +1187,25 @@
         <v>26</v>
       </c>
       <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
         <v>202</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2502</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>100</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>20000</v>
       </c>
@@ -1166,18 +1219,21 @@
         <v>27</v>
       </c>
       <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>165</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>3503</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>100</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1194,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8977B2-AAE5-4B3C-96B4-E86BDEB69204}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1207,13 +1263,14 @@
     <col min="3" max="3" width="8.84375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.61328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="36.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" customWidth="1"/>
+    <col min="7" max="7" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.61328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="36.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1230,257 +1287,147 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>250</v>
+      </c>
+      <c r="H2">
+        <v>3000</v>
+      </c>
+      <c r="I2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3">
+        <v>2500</v>
+      </c>
+      <c r="I3">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>180</v>
+      </c>
+      <c r="H4">
+        <v>3500</v>
+      </c>
+      <c r="I4">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>4096</v>
-      </c>
-      <c r="G5">
-        <v>4096</v>
-      </c>
-      <c r="H5">
-        <v>1000</v>
-      </c>
-      <c r="I5" s="2">
-        <v>255</v>
-      </c>
-      <c r="J5" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>233</v>
-      </c>
-      <c r="G6">
-        <v>2700</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>358</v>
-      </c>
-      <c r="G7">
-        <v>3600</v>
-      </c>
-      <c r="I7" s="2">
-        <v>255</v>
-      </c>
-      <c r="J7" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8">
-        <v>250</v>
-      </c>
-      <c r="G8">
-        <v>3000</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>10000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <v>200</v>
-      </c>
-      <c r="G9">
-        <v>2500</v>
-      </c>
-      <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>10000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10">
-        <v>180</v>
-      </c>
-      <c r="G10">
-        <v>3500</v>
-      </c>
-      <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.4">
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>